<commit_message>
inceput TOTAL stat salarii
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/downloads/Stat Salarii - Ingenio Software S.A. - Martie 2020.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/downloads/Stat Salarii - Ingenio Software S.A. - Martie 2020.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
   <si>
     <t xml:space="preserve">, </t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>SC</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -2394,74 +2397,169 @@
       </c>
       <c r="U26" s="50"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
-      <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
+    <row r="27">
+      <c r="A27" s="51"/>
+      <c r="B27" t="s" s="52">
+        <v>87</v>
+      </c>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="53" t="n">
+        <f>E15+E18+E21+E24</f>
+        <v>12159.0</v>
+      </c>
+      <c r="F27" t="n" s="52">
+        <v>8.0</v>
+      </c>
+      <c r="G27" s="54" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H27" s="52"/>
+      <c r="I27" t="n" s="52">
+        <v>0.0</v>
+      </c>
+      <c r="J27" t="n" s="52">
+        <v>0.0</v>
+      </c>
+      <c r="K27" t="n" s="52">
+        <v>0.0</v>
+      </c>
+      <c r="L27" s="53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M27" s="53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N27" s="53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O27" s="53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P27" s="53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q27" s="53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R27" t="n" s="52">
+        <v>0.0</v>
+      </c>
+      <c r="S27" s="53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T27" s="53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U27" s="55"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="47"/>
+      <c r="E28" s="40" t="n">
+        <f>E16+E19+E22+E25</f>
+        <v>0.0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L28" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M28" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N28" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O28" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P28" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q28" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R28" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S28" t="n" s="40">
+        <v>0.0</v>
+      </c>
+      <c r="T28" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U28" s="49"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="48"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="46" t="n">
+        <f>D17+D20+D23+D26</f>
+        <v>0.0</v>
+      </c>
+      <c r="E29" s="46" t="n">
+        <f>E17+E20+E23+E26</f>
+        <v>0.0</v>
+      </c>
+      <c r="F29" t="n" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="G29" t="n" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="H29" t="n" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="I29" t="n" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="J29" s="44"/>
+      <c r="K29" t="n" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L29" t="n" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="M29" s="46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N29" s="44"/>
+      <c r="O29" t="n" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="P29" s="46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q29" s="46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R29" t="n" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="S29" t="n" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="T29" s="46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U29" s="50"/>
     </row>
     <row r="30" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="16"/>
@@ -2509,7 +2607,7 @@
       <c r="T31" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="24">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
@@ -2532,6 +2630,8 @@
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="G24:H24"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="G27:H27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
started on tabel final
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/downloads/Stat Salarii - Ingenio Software S.A. - Martie 2020.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/downloads/Stat Salarii - Ingenio Software S.A. - Martie 2020.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="93">
   <si>
     <t xml:space="preserve">, </t>
   </si>
@@ -278,6 +278,21 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>OBLIGATII ANGAJATOR</t>
+  </si>
+  <si>
+    <t>BAZA DE CALCUL</t>
+  </si>
+  <si>
+    <t>CONTRIBUTIA</t>
+  </si>
+  <si>
+    <t>CALCULATA</t>
+  </si>
+  <si>
+    <t>DEFALCATE</t>
   </si>
 </sst>
 </file>
@@ -285,7 +300,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -315,15 +330,24 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="7"/>
       <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <sz val="7.0"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
     </font>
   </fonts>
   <fills count="5">
@@ -843,127 +867,127 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -972,6 +996,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -1021,6 +1046,22 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="48" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="38" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1307,483 +1348,483 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="13" width="3.7109375" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="13" width="14.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="29" width="13.42578125" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="34" width="7.7109375" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="34" width="11.140625" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="4.0" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="3.7109375" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="11.0" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="false"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="11.140625" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="7.140625" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="false"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="false"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="13.28515625" collapsed="false"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="false"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="false"/>
-    <col min="22" max="16384" style="13" width="9.140625" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="7" width="3.7109375" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="7" width="14.28515625" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="9" width="13.42578125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="7.7109375" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="11.140625" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="6" width="4.0" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="6" width="4.28515625" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="6" width="3.7109375" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="6" width="7.85546875" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="6" width="7.0" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="6" width="6.7109375" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="6" width="11.0" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="6" width="13.85546875" collapsed="false"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="6" width="11.140625" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="6" width="9.0" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="6" width="7.140625" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="6" width="5.42578125" collapsed="false"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="6" width="12.0" collapsed="false"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="6" width="13.28515625" collapsed="false"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="6" width="12.42578125" collapsed="false"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="6" width="9.85546875" collapsed="false"/>
+    <col min="22" max="16384" style="7" width="9.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="L4" s="22" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="L4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:21" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="L5" s="23" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="L5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="13">
+      <c r="A8" s="7">
         <v>0</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="7">
         <v>1</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="9">
         <v>2</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="5">
         <v>3</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="5">
         <v>4</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="6">
         <v>5</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="6">
         <v>6</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="6">
         <v>7</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="6">
         <v>8</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="6">
         <v>9</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="6">
         <v>10</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="6">
         <v>11</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="6">
         <v>12</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N8" s="6">
         <v>13</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="6">
         <v>14</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P8" s="6">
         <v>15</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Q8" s="6">
         <v>16</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8" s="6">
         <v>17</v>
       </c>
-      <c r="S8" s="1">
+      <c r="S8" s="6">
         <v>18</v>
       </c>
-      <c r="T8" s="1">
+      <c r="T8" s="6">
         <v>19</v>
       </c>
-      <c r="U8" s="1">
+      <c r="U8" s="6">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="35" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="35"/>
-      <c r="F9" s="5" t="s">
+      <c r="E9" s="12"/>
+      <c r="F9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="5" t="s">
+      <c r="H9" s="14"/>
+      <c r="I9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="O9" s="5" t="s">
+      <c r="O9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="P9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="5" t="s">
+      <c r="Q9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="R9" s="5" t="s">
+      <c r="R9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="S9" s="5" t="s">
+      <c r="S9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="T9" s="5" t="s">
+      <c r="T9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="U9" s="6" t="s">
+      <c r="U9" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="8">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="21">
         <v>0.75</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7" t="s">
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="P10" s="7" t="s">
+      <c r="P10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7" t="s">
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="U10" s="9"/>
+      <c r="U10" s="22"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="37" t="s">
+      <c r="C11" s="23"/>
+      <c r="D11" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="7" t="s">
+      <c r="E11" s="24"/>
+      <c r="F11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="K11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="L11" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="M11" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="N11" s="7" t="s">
+      <c r="N11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="7" t="s">
+      <c r="O11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="P11" s="7" t="s">
+      <c r="P11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="Q11" s="7" t="s">
+      <c r="Q11" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="R11" s="7" t="s">
+      <c r="R11" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="S11" s="7" t="s">
+      <c r="S11" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="T11" s="7" t="s">
+      <c r="T11" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="U11" s="9"/>
+      <c r="U11" s="22"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="37" t="s">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7" t="s">
+      <c r="E12" s="24"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7" t="s">
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="9"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="22"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="21"/>
-      <c r="L13" s="7" t="s">
+      <c r="K13" s="26"/>
+      <c r="L13" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="M13" s="7" t="s">
+      <c r="M13" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="N13" s="7" t="s">
+      <c r="N13" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="O13" s="7" t="s">
+      <c r="O13" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="P13" s="7" t="s">
+      <c r="P13" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="Q13" s="7" t="s">
+      <c r="Q13" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="R13" s="7" t="s">
+      <c r="R13" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="S13" s="7" t="s">
+      <c r="S13" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="T13" s="7" t="s">
+      <c r="T13" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="U13" s="9"/>
+      <c r="U13" s="22"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="33" t="s">
+      <c r="A14" s="27"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="11">
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="32">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="P14" s="10" t="s">
+      <c r="P14" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="Q14" s="10" t="s">
+      <c r="Q14" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="12"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="33"/>
     </row>
     <row r="15">
-      <c r="A15" t="n" s="52">
+      <c r="A15" t="n" s="53">
         <v>1.0</v>
       </c>
-      <c r="B15" t="s" s="53">
+      <c r="B15" t="s" s="54">
         <v>75</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="54" t="n">
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="55" t="n">
         <v>3000.0</v>
       </c>
-      <c r="F15" s="55" t="n">
+      <c r="F15" s="56" t="n">
         <v>8.0</v>
       </c>
-      <c r="G15" s="55" t="n">
+      <c r="G15" s="56" t="n">
         <v>22.0</v>
       </c>
-      <c r="H15" s="53"/>
-      <c r="I15" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J15" t="n" s="53">
-        <v>0.0</v>
-      </c>
-      <c r="K15" t="n" s="53">
+      <c r="H15" s="54"/>
+      <c r="I15" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J15" t="n" s="54">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n" s="54">
         <v>176.0</v>
       </c>
-      <c r="L15" s="54" t="n">
+      <c r="L15" s="55" t="n">
         <v>3000.0</v>
       </c>
-      <c r="M15" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N15" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O15" s="54" t="n">
+      <c r="M15" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N15" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O15" s="55" t="n">
         <v>220.0</v>
       </c>
-      <c r="P15" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q15" s="54" t="n">
+      <c r="P15" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q15" s="55" t="n">
         <v>750.0</v>
       </c>
-      <c r="R15" t="n" s="53">
-        <v>0.0</v>
-      </c>
-      <c r="S15" s="54" t="n">
+      <c r="R15" t="n" s="54">
+        <v>0.0</v>
+      </c>
+      <c r="S15" s="55" t="n">
         <v>198.0</v>
       </c>
-      <c r="T15" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U15" s="56"/>
+      <c r="T15" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U15" s="57"/>
     </row>
     <row r="16">
-      <c r="A16" s="48"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="41" t="s">
         <v>76</v>
       </c>
@@ -1835,124 +1876,124 @@
       <c r="T16" s="40" t="n">
         <v>0.0</v>
       </c>
-      <c r="U16" s="50"/>
+      <c r="U16" s="51"/>
     </row>
     <row r="17">
-      <c r="A17" s="49"/>
-      <c r="B17" t="s" s="44">
+      <c r="A17" s="50"/>
+      <c r="B17" t="s" s="45">
         <v>76</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="D17" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="E17" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="F17" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G17" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H17" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I17" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J17" s="44"/>
-      <c r="K17" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="L17" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="M17" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N17" s="44"/>
-      <c r="O17" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="P17" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q17" s="47" t="n">
+      <c r="D17" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="E17" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="F17" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G17" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H17" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I17" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J17" s="45"/>
+      <c r="K17" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="L17" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M17" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N17" s="45"/>
+      <c r="O17" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="P17" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q17" s="48" t="n">
         <v>195.0</v>
       </c>
-      <c r="R17" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="S17" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="T17" s="47" t="n">
+      <c r="R17" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="S17" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="T17" s="48" t="n">
         <v>1753.0</v>
       </c>
-      <c r="U17" s="51"/>
+      <c r="U17" s="52"/>
     </row>
     <row r="18">
-      <c r="A18" t="n" s="52">
+      <c r="A18" t="n" s="53">
         <v>2.0</v>
       </c>
-      <c r="B18" t="s" s="53">
+      <c r="B18" t="s" s="54">
         <v>78</v>
       </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="54" t="n">
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="55" t="n">
         <v>1197.0</v>
       </c>
-      <c r="F18" s="55" t="n">
+      <c r="F18" s="56" t="n">
         <v>8.0</v>
       </c>
-      <c r="G18" s="55" t="n">
+      <c r="G18" s="56" t="n">
         <v>22.0</v>
       </c>
-      <c r="H18" s="53"/>
-      <c r="I18" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J18" t="n" s="53">
-        <v>0.0</v>
-      </c>
-      <c r="K18" t="n" s="53">
+      <c r="H18" s="54"/>
+      <c r="I18" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J18" t="n" s="54">
+        <v>0.0</v>
+      </c>
+      <c r="K18" t="n" s="54">
         <v>44.0</v>
       </c>
-      <c r="L18" s="54" t="n">
+      <c r="L18" s="55" t="n">
         <v>1197.0</v>
       </c>
-      <c r="M18" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N18" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O18" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P18" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q18" s="54" t="n">
+      <c r="M18" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N18" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O18" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P18" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q18" s="55" t="n">
         <v>299.0</v>
       </c>
-      <c r="R18" t="n" s="53">
-        <v>0.0</v>
-      </c>
-      <c r="S18" s="54" t="n">
+      <c r="R18" t="n" s="54">
+        <v>0.0</v>
+      </c>
+      <c r="S18" s="55" t="n">
         <v>78.0</v>
       </c>
-      <c r="T18" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U18" s="56"/>
+      <c r="T18" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U18" s="57"/>
     </row>
     <row r="19">
-      <c r="A19" s="48"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="41" t="s">
         <v>79</v>
       </c>
@@ -2004,124 +2045,124 @@
       <c r="T19" s="40" t="n">
         <v>0.0</v>
       </c>
-      <c r="U19" s="50"/>
+      <c r="U19" s="51"/>
     </row>
     <row r="20">
-      <c r="A20" s="49"/>
-      <c r="B20" t="s" s="44">
+      <c r="A20" s="50"/>
+      <c r="B20" t="s" s="45">
         <v>76</v>
       </c>
-      <c r="C20" s="45" t="s">
+      <c r="C20" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="D20" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="E20" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="F20" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G20" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H20" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I20" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J20" s="44"/>
-      <c r="K20" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="L20" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="M20" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N20" s="44"/>
-      <c r="O20" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="P20" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q20" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R20" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="S20" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="T20" s="47" t="n">
+      <c r="D20" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="E20" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="F20" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G20" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H20" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I20" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J20" s="45"/>
+      <c r="K20" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="L20" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M20" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N20" s="45"/>
+      <c r="O20" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="P20" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q20" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R20" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="S20" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="T20" s="48" t="n">
         <v>700.0</v>
       </c>
-      <c r="U20" s="51"/>
+      <c r="U20" s="52"/>
     </row>
     <row r="21">
-      <c r="A21" t="n" s="52">
+      <c r="A21" t="n" s="53">
         <v>3.0</v>
       </c>
-      <c r="B21" t="s" s="53">
+      <c r="B21" t="s" s="54">
         <v>81</v>
       </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="54" t="n">
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="55" t="n">
         <v>2508.0</v>
       </c>
-      <c r="F21" s="55" t="n">
+      <c r="F21" s="56" t="n">
         <v>8.0</v>
       </c>
-      <c r="G21" s="55" t="n">
+      <c r="G21" s="56" t="n">
         <v>22.0</v>
       </c>
-      <c r="H21" s="53"/>
-      <c r="I21" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J21" t="n" s="53">
-        <v>0.0</v>
-      </c>
-      <c r="K21" t="n" s="53">
+      <c r="H21" s="54"/>
+      <c r="I21" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J21" t="n" s="54">
+        <v>0.0</v>
+      </c>
+      <c r="K21" t="n" s="54">
         <v>176.0</v>
       </c>
-      <c r="L21" s="54" t="n">
+      <c r="L21" s="55" t="n">
         <v>2508.0</v>
       </c>
-      <c r="M21" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N21" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O21" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P21" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q21" s="54" t="n">
+      <c r="M21" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N21" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O21" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P21" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q21" s="55" t="n">
         <v>627.0</v>
       </c>
-      <c r="R21" t="n" s="53">
-        <v>0.0</v>
-      </c>
-      <c r="S21" s="54" t="n">
+      <c r="R21" t="n" s="54">
+        <v>0.0</v>
+      </c>
+      <c r="S21" s="55" t="n">
         <v>130.0</v>
       </c>
-      <c r="T21" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U21" s="56"/>
+      <c r="T21" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U21" s="57"/>
     </row>
     <row r="22">
-      <c r="A22" s="48"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="41" t="s">
         <v>82</v>
       </c>
@@ -2173,124 +2214,124 @@
       <c r="T22" s="40" t="n">
         <v>0.0</v>
       </c>
-      <c r="U22" s="50"/>
+      <c r="U22" s="51"/>
     </row>
     <row r="23">
-      <c r="A23" s="49"/>
-      <c r="B23" t="s" s="44">
+      <c r="A23" s="50"/>
+      <c r="B23" t="s" s="45">
         <v>76</v>
       </c>
-      <c r="C23" s="45" t="s">
+      <c r="C23" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="D23" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="E23" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="F23" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G23" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H23" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I23" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J23" s="44"/>
-      <c r="K23" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="L23" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="M23" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N23" s="44"/>
-      <c r="O23" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="P23" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q23" s="47" t="n">
+      <c r="D23" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="E23" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="F23" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G23" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H23" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I23" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J23" s="45"/>
+      <c r="K23" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="L23" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M23" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N23" s="45"/>
+      <c r="O23" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="P23" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q23" s="48" t="n">
         <v>330.0</v>
       </c>
-      <c r="R23" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="S23" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="T23" s="47" t="n">
+      <c r="R23" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="S23" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="T23" s="48" t="n">
         <v>1500.0</v>
       </c>
-      <c r="U23" s="51"/>
+      <c r="U23" s="52"/>
     </row>
     <row r="24">
-      <c r="A24" t="n" s="52">
+      <c r="A24" t="n" s="53">
         <v>4.0</v>
       </c>
-      <c r="B24" t="s" s="53">
+      <c r="B24" t="s" s="54">
         <v>84</v>
       </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="54" t="n">
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="55" t="n">
         <v>5454.0</v>
       </c>
-      <c r="F24" s="55" t="n">
+      <c r="F24" s="56" t="n">
         <v>8.0</v>
       </c>
-      <c r="G24" s="55" t="n">
+      <c r="G24" s="56" t="n">
         <v>20.0</v>
       </c>
-      <c r="H24" s="53"/>
-      <c r="I24" s="55" t="n">
+      <c r="H24" s="54"/>
+      <c r="I24" s="56" t="n">
         <v>2.0</v>
       </c>
-      <c r="J24" t="n" s="53">
-        <v>0.0</v>
-      </c>
-      <c r="K24" t="n" s="53">
+      <c r="J24" t="n" s="54">
+        <v>0.0</v>
+      </c>
+      <c r="K24" t="n" s="54">
         <v>160.0</v>
       </c>
-      <c r="L24" s="54" t="n">
+      <c r="L24" s="55" t="n">
         <v>4958.0</v>
       </c>
-      <c r="M24" s="54" t="n">
+      <c r="M24" s="55" t="n">
         <v>349.0</v>
       </c>
-      <c r="N24" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O24" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P24" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q24" s="54" t="n">
+      <c r="N24" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O24" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P24" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q24" s="55" t="n">
         <v>1327.0</v>
       </c>
-      <c r="R24" t="n" s="53">
-        <v>0.0</v>
-      </c>
-      <c r="S24" s="54" t="n">
+      <c r="R24" t="n" s="54">
+        <v>0.0</v>
+      </c>
+      <c r="S24" s="55" t="n">
         <v>348.0</v>
       </c>
-      <c r="T24" s="54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U24" s="56"/>
+      <c r="T24" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U24" s="57"/>
     </row>
     <row r="25">
-      <c r="A25" s="48"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="41" t="s">
         <v>85</v>
       </c>
@@ -2342,134 +2383,134 @@
       <c r="T25" s="40" t="n">
         <v>0.0</v>
       </c>
-      <c r="U25" s="50"/>
+      <c r="U25" s="51"/>
     </row>
     <row r="26">
-      <c r="A26" s="49"/>
-      <c r="B26" t="s" s="44">
+      <c r="A26" s="50"/>
+      <c r="B26" t="s" s="45">
         <v>76</v>
       </c>
-      <c r="C26" s="45" t="s">
+      <c r="C26" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="D26" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="E26" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="F26" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G26" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H26" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I26" s="46" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J26" s="44"/>
-      <c r="K26" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="L26" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="M26" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N26" s="44"/>
-      <c r="O26" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="P26" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q26" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R26" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="S26" t="n" s="44">
-        <v>0.0</v>
-      </c>
-      <c r="T26" s="47" t="n">
+      <c r="D26" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="E26" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="F26" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G26" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H26" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I26" s="47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J26" s="45"/>
+      <c r="K26" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="L26" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M26" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N26" s="45"/>
+      <c r="O26" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="P26" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q26" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R26" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="S26" t="n" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="T26" s="48" t="n">
         <v>3136.0</v>
       </c>
-      <c r="U26" s="51"/>
+      <c r="U26" s="52"/>
     </row>
     <row r="27">
-      <c r="A27" s="52"/>
-      <c r="B27" t="s" s="53">
+      <c r="A27" s="53"/>
+      <c r="B27" t="s" s="54">
         <v>87</v>
       </c>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="54" t="n">
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="55" t="n">
         <f>E15+E18+E21+E24</f>
         <v>12159.0</v>
       </c>
-      <c r="F27" s="53"/>
-      <c r="G27" s="55" t="n">
+      <c r="F27" s="54"/>
+      <c r="G27" s="56" t="n">
         <f>G15+G18+G21+G24</f>
         <v>86.0</v>
       </c>
-      <c r="H27" s="53"/>
-      <c r="I27" s="55" t="n">
+      <c r="H27" s="54"/>
+      <c r="I27" s="56" t="n">
         <f>I15+I18+I21+I24</f>
         <v>2.0</v>
       </c>
-      <c r="J27" t="n" s="53">
+      <c r="J27" t="n" s="54">
         <f>J15+J18+J21+J24</f>
         <v>0.0</v>
       </c>
-      <c r="K27" t="n" s="53">
+      <c r="K27" t="n" s="54">
         <f>K15+K18+K21+K24</f>
         <v>556.0</v>
       </c>
-      <c r="L27" s="54" t="n">
+      <c r="L27" s="55" t="n">
         <f>L15+L18+L21+L24</f>
         <v>11663.0</v>
       </c>
-      <c r="M27" s="54" t="n">
+      <c r="M27" s="55" t="n">
         <f>M15+M18+M21+M24</f>
         <v>349.0</v>
       </c>
-      <c r="N27" s="54" t="n">
+      <c r="N27" s="55" t="n">
         <f>N15+N18+N21+N24</f>
         <v>0.0</v>
       </c>
-      <c r="O27" s="54" t="n">
+      <c r="O27" s="55" t="n">
         <f>O15+O18+O21+O24</f>
         <v>220.0</v>
       </c>
-      <c r="P27" s="54" t="n">
+      <c r="P27" s="55" t="n">
         <f>P15+P18+P21+P24</f>
         <v>0.0</v>
       </c>
-      <c r="Q27" s="54" t="n">
+      <c r="Q27" s="55" t="n">
         <f>Q15+Q18+Q21+Q24</f>
         <v>3003.0</v>
       </c>
-      <c r="R27" t="n" s="53">
+      <c r="R27" t="n" s="54">
         <f>R15+R18+R21+R24</f>
         <v>0.0</v>
       </c>
-      <c r="S27" s="54" t="n">
-        <f>S16+S19+S22+S25</f>
-        <v>7089.0</v>
-      </c>
-      <c r="T27" s="54" t="n">
+      <c r="S27" s="55" t="n">
+        <f>S15+S18+S21+S24</f>
+        <v>754.0</v>
+      </c>
+      <c r="T27" s="55" t="n">
         <f>T15+T18+T21+T24</f>
         <v>0.0</v>
       </c>
-      <c r="U27" s="56"/>
+      <c r="U27" s="57"/>
     </row>
     <row r="28">
-      <c r="A28" s="48"/>
+      <c r="A28" s="49"/>
       <c r="E28" s="40" t="n">
         <f>E16+E19+E22+E25</f>
         <v>0.0</v>
@@ -2530,128 +2571,163 @@
         <f>T16+T19+T22+T25</f>
         <v>0.0</v>
       </c>
-      <c r="U28" s="50"/>
+      <c r="U28" s="51"/>
     </row>
     <row r="29">
-      <c r="A29" s="49"/>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="47" t="n">
+      <c r="A29" s="50"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="48" t="n">
         <f>D17+D20+D23+D26</f>
         <v>0.0</v>
       </c>
-      <c r="E29" s="47" t="n">
+      <c r="E29" s="48" t="n">
         <f>E17+E20+E23+E26</f>
         <v>0.0</v>
       </c>
-      <c r="F29" s="46" t="n">
+      <c r="F29" s="47" t="n">
         <f>F17+F20+F23+F26</f>
         <v>0.0</v>
       </c>
-      <c r="G29" s="46" t="n">
+      <c r="G29" s="47" t="n">
         <f>G17+G20+G23+G26</f>
         <v>0.0</v>
       </c>
-      <c r="H29" s="46" t="n">
+      <c r="H29" s="47" t="n">
         <f>H17+H20+H23+H26</f>
         <v>0.0</v>
       </c>
-      <c r="I29" s="46" t="n">
+      <c r="I29" s="47" t="n">
         <f>I17+I20+I23+I26</f>
         <v>0.0</v>
       </c>
-      <c r="J29" s="44"/>
-      <c r="K29" t="n" s="44">
+      <c r="J29" s="45"/>
+      <c r="K29" t="n" s="45">
         <f>K17+K20+K23+K26</f>
         <v>0.0</v>
       </c>
-      <c r="L29" t="n" s="44">
+      <c r="L29" t="n" s="45">
         <f>L17+L20+L23+L26</f>
         <v>0.0</v>
       </c>
-      <c r="M29" s="47" t="n">
+      <c r="M29" s="48" t="n">
         <f>N17+N20+N23+N26</f>
         <v>0.0</v>
       </c>
-      <c r="N29" s="44"/>
-      <c r="O29" t="n" s="44">
+      <c r="N29" s="45"/>
+      <c r="O29" t="n" s="45">
         <f>O17+O20+O23+O26</f>
         <v>0.0</v>
       </c>
-      <c r="P29" s="47" t="n">
+      <c r="P29" s="48" t="n">
         <f>P17+P20+P23+P26</f>
         <v>0.0</v>
       </c>
-      <c r="Q29" s="47" t="n">
+      <c r="Q29" s="48" t="n">
         <f>Q17+Q20+Q23+Q26</f>
         <v>525.0</v>
       </c>
-      <c r="R29" t="n" s="44">
+      <c r="R29" t="n" s="45">
         <f>R17+R20+R23+R26</f>
         <v>0.0</v>
       </c>
-      <c r="S29" s="47" t="n">
+      <c r="S29" s="48" t="n">
         <f>S17+S20+S23+S26</f>
         <v>0.0</v>
       </c>
-      <c r="T29" s="47" t="n">
+      <c r="T29" s="48" t="n">
         <f>T17+T20+T23+T26</f>
         <v>7089.0</v>
       </c>
-      <c r="U29" s="51"/>
+      <c r="U29" s="52"/>
     </row>
     <row r="30" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="39"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="39"/>
+      <c r="Q30" s="39"/>
+      <c r="R30" s="39"/>
+      <c r="S30" s="39"/>
+      <c r="T30" s="39"/>
+      <c r="U30" s="39"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="54"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="J31" s="54"/>
+      <c r="K31" s="57"/>
+      <c r="M31" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="N31" s="54"/>
+      <c r="O31" s="54"/>
+      <c r="P31" s="57"/>
+      <c r="Q31" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="R31" s="54"/>
+      <c r="S31" s="57"/>
+      <c r="T31" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="U31" s="57"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="50"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="J32" s="45"/>
+      <c r="K32" s="52"/>
+      <c r="M32" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="N32" s="45"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="52"/>
+      <c r="Q32" s="50"/>
+      <c r="R32" s="45"/>
+      <c r="S32" s="52"/>
+      <c r="T32" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="U32" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
+  <mergeCells count="63">
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="D11:E11"/>
@@ -2661,6 +2737,11 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="G9:H9"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="B18:C18"/>
@@ -2671,6 +2752,45 @@
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="G27:H27"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="M31:P31"/>
+    <mergeCell ref="M32:P32"/>
+    <mergeCell ref="M33:P33"/>
+    <mergeCell ref="M34:P34"/>
+    <mergeCell ref="Q31:S31"/>
+    <mergeCell ref="Q33:S33"/>
+    <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="T32:U32"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="L38:N38"/>
+    <mergeCell ref="L39:N39"/>
+    <mergeCell ref="O38:Q38"/>
+    <mergeCell ref="O39:Q39"/>
+    <mergeCell ref="R38:T38"/>
+    <mergeCell ref="R39:T39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
stat salarii?? +buton de reset calcul la Realizariretineri.js
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/downloads/Stat Salarii - Ingenio Software S.A. - Martie 2020.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/downloads/Stat Salarii - Ingenio Software S.A. - Martie 2020.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="106">
   <si>
     <t xml:space="preserve">, </t>
   </si>
@@ -283,6 +283,18 @@
     <t>OBLIGATII ANGAJATOR</t>
   </si>
   <si>
+    <t>CAS cond. Speciale/Deosebite</t>
+  </si>
+  <si>
+    <t>Contributie CAM 2.25%</t>
+  </si>
+  <si>
+    <t>Contributie CAM 0.3375%***</t>
+  </si>
+  <si>
+    <t>Fond 4% pers cu handicap</t>
+  </si>
+  <si>
     <t>BAZA DE CALCUL</t>
   </si>
   <si>
@@ -293,6 +305,33 @@
   </si>
   <si>
     <t>DEFALCATE</t>
+  </si>
+  <si>
+    <t>CAS cond speciale 8%</t>
+  </si>
+  <si>
+    <t>CAS cond speciale 4%</t>
+  </si>
+  <si>
+    <t>RECAPITULARE SALARIATI</t>
+  </si>
+  <si>
+    <t>Total retineri salariati</t>
+  </si>
+  <si>
+    <t>CAS 25%***</t>
+  </si>
+  <si>
+    <t>CAS 21.25%***</t>
+  </si>
+  <si>
+    <t>CAS 10%***</t>
+  </si>
+  <si>
+    <t>CAS scutit***</t>
+  </si>
+  <si>
+    <t>Impozit scutit cf. art. 60 din CF</t>
   </si>
 </sst>
 </file>
@@ -372,7 +411,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="64">
     <border>
       <left/>
       <right/>
@@ -863,11 +902,151 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -997,6 +1176,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -1062,6 +1242,30 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="53" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="58" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="63" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="4" borderId="13" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="4" borderId="23" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="4" borderId="53" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1348,7 +1552,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U32"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
@@ -1767,64 +1971,64 @@
       <c r="U14" s="33"/>
     </row>
     <row r="15">
-      <c r="A15" t="n" s="53">
+      <c r="A15" t="n" s="54">
         <v>1.0</v>
       </c>
-      <c r="B15" t="s" s="54">
+      <c r="B15" t="s" s="55">
         <v>75</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="55" t="n">
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="56" t="n">
         <v>3000.0</v>
       </c>
-      <c r="F15" s="56" t="n">
+      <c r="F15" s="57" t="n">
         <v>8.0</v>
       </c>
-      <c r="G15" s="56" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="H15" s="54"/>
-      <c r="I15" s="56" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J15" t="n" s="54">
-        <v>0.0</v>
-      </c>
-      <c r="K15" t="n" s="54">
-        <v>176.0</v>
-      </c>
-      <c r="L15" s="55" t="n">
-        <v>3000.0</v>
-      </c>
-      <c r="M15" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N15" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O15" s="55" t="n">
-        <v>220.0</v>
-      </c>
-      <c r="P15" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q15" s="55" t="n">
-        <v>750.0</v>
-      </c>
-      <c r="R15" t="n" s="54">
-        <v>0.0</v>
-      </c>
-      <c r="S15" s="55" t="n">
-        <v>198.0</v>
-      </c>
-      <c r="T15" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U15" s="57"/>
+      <c r="G15" s="57" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="H15" s="55"/>
+      <c r="I15" s="57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J15" t="n" s="55">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n" s="55">
+        <v>80.0</v>
+      </c>
+      <c r="L15" s="56" t="n">
+        <v>1364.0</v>
+      </c>
+      <c r="M15" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N15" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O15" s="56" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="P15" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q15" s="56" t="n">
+        <v>341.0</v>
+      </c>
+      <c r="R15" t="n" s="55">
+        <v>0.0</v>
+      </c>
+      <c r="S15" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T15" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U15" s="58"/>
     </row>
     <row r="16">
-      <c r="A16" s="49"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="41" t="s">
         <v>76</v>
       </c>
@@ -1850,7 +2054,7 @@
         <v>0.0</v>
       </c>
       <c r="L16" s="40" t="n">
-        <v>0.0</v>
+        <v>1636.363525390625</v>
       </c>
       <c r="M16" s="40" t="n">
         <v>0.0</v>
@@ -1859,141 +2063,141 @@
         <v>0.0</v>
       </c>
       <c r="O16" s="40" t="n">
-        <v>3000.0</v>
+        <v>1364.0</v>
       </c>
       <c r="P16" s="40" t="n">
         <v>0.0</v>
       </c>
       <c r="Q16" s="40" t="n">
-        <v>300.0</v>
+        <v>136.0</v>
       </c>
       <c r="R16" s="40" t="n">
-        <v>1753.0</v>
+        <v>887.0</v>
       </c>
       <c r="S16" t="n" s="40">
-        <v>1753.0</v>
+        <v>887.0</v>
       </c>
       <c r="T16" s="40" t="n">
         <v>0.0</v>
       </c>
-      <c r="U16" s="51"/>
+      <c r="U16" s="52"/>
     </row>
     <row r="17">
-      <c r="A17" s="50"/>
-      <c r="B17" t="s" s="45">
+      <c r="A17" s="51"/>
+      <c r="B17" t="s" s="46">
         <v>76</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="D17" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="E17" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="F17" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G17" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H17" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I17" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J17" s="45"/>
-      <c r="K17" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="L17" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="M17" s="48" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N17" s="45"/>
-      <c r="O17" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="P17" s="48" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q17" s="48" t="n">
-        <v>195.0</v>
-      </c>
-      <c r="R17" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="S17" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="T17" s="48" t="n">
-        <v>1753.0</v>
-      </c>
-      <c r="U17" s="52"/>
+      <c r="D17" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="E17" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="F17" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G17" s="48" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H17" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I17" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J17" s="46"/>
+      <c r="K17" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="L17" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="M17" s="49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N17" s="46"/>
+      <c r="O17" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="P17" s="49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q17" s="49" t="n">
+        <v>510.0</v>
+      </c>
+      <c r="R17" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="S17" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="T17" s="49" t="n">
+        <v>887.0</v>
+      </c>
+      <c r="U17" s="53"/>
     </row>
     <row r="18">
-      <c r="A18" t="n" s="53">
+      <c r="A18" t="n" s="54">
         <v>2.0</v>
       </c>
-      <c r="B18" t="s" s="54">
+      <c r="B18" t="s" s="55">
         <v>78</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="55" t="n">
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56" t="n">
         <v>1197.0</v>
       </c>
-      <c r="F18" s="56" t="n">
+      <c r="F18" s="57" t="n">
         <v>8.0</v>
       </c>
-      <c r="G18" s="56" t="n">
+      <c r="G18" s="57" t="n">
         <v>22.0</v>
       </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="56" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J18" t="n" s="54">
-        <v>0.0</v>
-      </c>
-      <c r="K18" t="n" s="54">
+      <c r="H18" s="55"/>
+      <c r="I18" s="57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J18" t="n" s="55">
+        <v>0.0</v>
+      </c>
+      <c r="K18" t="n" s="55">
         <v>44.0</v>
       </c>
-      <c r="L18" s="55" t="n">
+      <c r="L18" s="56" t="n">
         <v>1197.0</v>
       </c>
-      <c r="M18" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N18" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O18" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P18" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q18" s="55" t="n">
+      <c r="M18" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N18" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O18" s="56" t="n">
+        <v>220.0</v>
+      </c>
+      <c r="P18" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q18" s="56" t="n">
         <v>299.0</v>
       </c>
-      <c r="R18" t="n" s="54">
-        <v>0.0</v>
-      </c>
-      <c r="S18" s="55" t="n">
-        <v>78.0</v>
-      </c>
-      <c r="T18" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U18" s="57"/>
+      <c r="R18" t="n" s="55">
+        <v>0.0</v>
+      </c>
+      <c r="S18" s="56" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="T18" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U18" s="58"/>
     </row>
     <row r="19">
-      <c r="A19" s="49"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="41" t="s">
         <v>79</v>
       </c>
@@ -2037,132 +2241,132 @@
         <v>120.0</v>
       </c>
       <c r="R19" s="40" t="n">
-        <v>700.0</v>
+        <v>678.0</v>
       </c>
       <c r="S19" t="n" s="40">
-        <v>700.0</v>
+        <v>678.0</v>
       </c>
       <c r="T19" s="40" t="n">
         <v>0.0</v>
       </c>
-      <c r="U19" s="51"/>
+      <c r="U19" s="52"/>
     </row>
     <row r="20">
-      <c r="A20" s="50"/>
-      <c r="B20" t="s" s="45">
+      <c r="A20" s="51"/>
+      <c r="B20" t="s" s="46">
         <v>76</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="D20" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="E20" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="F20" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G20" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H20" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I20" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J20" s="45"/>
-      <c r="K20" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="L20" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="M20" s="48" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N20" s="45"/>
-      <c r="O20" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="P20" s="48" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q20" s="48" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R20" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="S20" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="T20" s="48" t="n">
-        <v>700.0</v>
-      </c>
-      <c r="U20" s="52"/>
+      <c r="D20" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="E20" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="F20" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G20" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H20" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I20" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J20" s="46"/>
+      <c r="K20" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="L20" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="M20" s="49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N20" s="46"/>
+      <c r="O20" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="P20" s="49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q20" s="49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R20" t="n" s="46">
+        <v>998.0</v>
+      </c>
+      <c r="S20" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="T20" s="49" t="n">
+        <v>678.0</v>
+      </c>
+      <c r="U20" s="53"/>
     </row>
     <row r="21">
-      <c r="A21" t="n" s="53">
+      <c r="A21" t="n" s="54">
         <v>3.0</v>
       </c>
-      <c r="B21" t="s" s="54">
+      <c r="B21" t="s" s="55">
         <v>81</v>
       </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="55" t="n">
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56" t="n">
         <v>2508.0</v>
       </c>
-      <c r="F21" s="56" t="n">
+      <c r="F21" s="57" t="n">
         <v>8.0</v>
       </c>
-      <c r="G21" s="56" t="n">
+      <c r="G21" s="57" t="n">
         <v>22.0</v>
       </c>
-      <c r="H21" s="54"/>
-      <c r="I21" s="56" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J21" t="n" s="54">
-        <v>0.0</v>
-      </c>
-      <c r="K21" t="n" s="54">
+      <c r="H21" s="55"/>
+      <c r="I21" s="57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J21" t="n" s="55">
+        <v>0.0</v>
+      </c>
+      <c r="K21" t="n" s="55">
         <v>176.0</v>
       </c>
-      <c r="L21" s="55" t="n">
+      <c r="L21" s="56" t="n">
         <v>2508.0</v>
       </c>
-      <c r="M21" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N21" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O21" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P21" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q21" s="55" t="n">
+      <c r="M21" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N21" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O21" s="56" t="n">
+        <v>220.0</v>
+      </c>
+      <c r="P21" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q21" s="56" t="n">
         <v>627.0</v>
       </c>
-      <c r="R21" t="n" s="54">
-        <v>0.0</v>
-      </c>
-      <c r="S21" s="55" t="n">
-        <v>130.0</v>
-      </c>
-      <c r="T21" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U21" s="57"/>
+      <c r="R21" t="n" s="55">
+        <v>0.0</v>
+      </c>
+      <c r="S21" s="56" t="n">
+        <v>152.0</v>
+      </c>
+      <c r="T21" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U21" s="58"/>
     </row>
     <row r="22">
-      <c r="A22" s="49"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="41" t="s">
         <v>82</v>
       </c>
@@ -2206,132 +2410,132 @@
         <v>251.0</v>
       </c>
       <c r="R22" s="40" t="n">
-        <v>1500.0</v>
+        <v>1478.0</v>
       </c>
       <c r="S22" t="n" s="40">
-        <v>1500.0</v>
+        <v>1478.0</v>
       </c>
       <c r="T22" s="40" t="n">
         <v>0.0</v>
       </c>
-      <c r="U22" s="51"/>
+      <c r="U22" s="52"/>
     </row>
     <row r="23">
-      <c r="A23" s="50"/>
-      <c r="B23" t="s" s="45">
+      <c r="A23" s="51"/>
+      <c r="B23" t="s" s="46">
         <v>76</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="D23" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="E23" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="F23" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G23" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H23" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I23" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J23" s="45"/>
-      <c r="K23" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="L23" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="M23" s="48" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N23" s="45"/>
-      <c r="O23" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="P23" s="48" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q23" s="48" t="n">
+      <c r="D23" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="E23" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="F23" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G23" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H23" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I23" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J23" s="46"/>
+      <c r="K23" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="L23" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="M23" s="49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N23" s="46"/>
+      <c r="O23" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="P23" s="49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q23" s="49" t="n">
         <v>330.0</v>
       </c>
-      <c r="R23" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="S23" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="T23" s="48" t="n">
-        <v>1500.0</v>
-      </c>
-      <c r="U23" s="52"/>
+      <c r="R23" t="n" s="46">
+        <v>1520.0</v>
+      </c>
+      <c r="S23" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="T23" s="49" t="n">
+        <v>1478.0</v>
+      </c>
+      <c r="U23" s="53"/>
     </row>
     <row r="24">
-      <c r="A24" t="n" s="53">
+      <c r="A24" t="n" s="54">
         <v>4.0</v>
       </c>
-      <c r="B24" t="s" s="54">
+      <c r="B24" t="s" s="55">
         <v>84</v>
       </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="55" t="n">
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="56" t="n">
         <v>5454.0</v>
       </c>
-      <c r="F24" s="56" t="n">
+      <c r="F24" s="57" t="n">
         <v>8.0</v>
       </c>
-      <c r="G24" s="56" t="n">
+      <c r="G24" s="57" t="n">
         <v>20.0</v>
       </c>
-      <c r="H24" s="54"/>
-      <c r="I24" s="56" t="n">
+      <c r="H24" s="55"/>
+      <c r="I24" s="57" t="n">
         <v>2.0</v>
       </c>
-      <c r="J24" t="n" s="54">
-        <v>0.0</v>
-      </c>
-      <c r="K24" t="n" s="54">
+      <c r="J24" t="n" s="55">
+        <v>0.0</v>
+      </c>
+      <c r="K24" t="n" s="55">
         <v>160.0</v>
       </c>
-      <c r="L24" s="55" t="n">
+      <c r="L24" s="56" t="n">
         <v>4958.0</v>
       </c>
-      <c r="M24" s="55" t="n">
-        <v>349.0</v>
-      </c>
-      <c r="N24" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="O24" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P24" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q24" s="55" t="n">
-        <v>1327.0</v>
-      </c>
-      <c r="R24" t="n" s="54">
-        <v>0.0</v>
-      </c>
-      <c r="S24" s="55" t="n">
-        <v>348.0</v>
-      </c>
-      <c r="T24" s="55" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U24" s="57"/>
+      <c r="M24" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N24" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O24" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P24" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q24" s="56" t="n">
+        <v>1240.0</v>
+      </c>
+      <c r="R24" t="n" s="55">
+        <v>0.0</v>
+      </c>
+      <c r="S24" s="56" t="n">
+        <v>322.0</v>
+      </c>
+      <c r="T24" s="56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U24" s="58"/>
     </row>
     <row r="25">
-      <c r="A25" s="49"/>
+      <c r="A25" s="50"/>
       <c r="B25" s="41" t="s">
         <v>85</v>
       </c>
@@ -2366,7 +2570,7 @@
         <v>0.0</v>
       </c>
       <c r="O25" s="40" t="n">
-        <v>5307.0</v>
+        <v>4958.0</v>
       </c>
       <c r="P25" s="40" t="n">
         <v>0.0</v>
@@ -2375,142 +2579,142 @@
         <v>496.0</v>
       </c>
       <c r="R25" s="40" t="n">
-        <v>3136.0</v>
+        <v>2900.0</v>
       </c>
       <c r="S25" t="n" s="40">
-        <v>3136.0</v>
+        <v>2900.0</v>
       </c>
       <c r="T25" s="40" t="n">
         <v>0.0</v>
       </c>
-      <c r="U25" s="51"/>
+      <c r="U25" s="52"/>
     </row>
     <row r="26">
-      <c r="A26" s="50"/>
-      <c r="B26" t="s" s="45">
+      <c r="A26" s="51"/>
+      <c r="B26" t="s" s="46">
         <v>76</v>
       </c>
-      <c r="C26" s="46" t="s">
+      <c r="C26" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="D26" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="E26" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="F26" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G26" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H26" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I26" s="47" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J26" s="45"/>
-      <c r="K26" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="L26" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="M26" s="48" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N26" s="45"/>
-      <c r="O26" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="P26" s="48" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q26" s="48" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R26" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="S26" t="n" s="45">
-        <v>0.0</v>
-      </c>
-      <c r="T26" s="48" t="n">
-        <v>3136.0</v>
-      </c>
-      <c r="U26" s="52"/>
+      <c r="D26" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="E26" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="F26" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G26" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H26" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I26" s="48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J26" s="46"/>
+      <c r="K26" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="L26" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="M26" s="49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N26" s="46"/>
+      <c r="O26" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="P26" s="49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q26" s="49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R26" t="n" s="46">
+        <v>3222.0</v>
+      </c>
+      <c r="S26" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="T26" s="49" t="n">
+        <v>2900.0</v>
+      </c>
+      <c r="U26" s="53"/>
     </row>
     <row r="27">
-      <c r="A27" s="53"/>
-      <c r="B27" t="s" s="54">
+      <c r="A27" s="54"/>
+      <c r="B27" t="s" s="55">
         <v>87</v>
       </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="55" t="n">
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="56" t="n">
         <f>E15+E18+E21+E24</f>
         <v>12159.0</v>
       </c>
-      <c r="F27" s="54"/>
-      <c r="G27" s="56" t="n">
+      <c r="F27" s="55"/>
+      <c r="G27" s="57" t="n">
         <f>G15+G18+G21+G24</f>
-        <v>86.0</v>
-      </c>
-      <c r="H27" s="54"/>
-      <c r="I27" s="56" t="n">
+        <v>74.0</v>
+      </c>
+      <c r="H27" s="55"/>
+      <c r="I27" s="57" t="n">
         <f>I15+I18+I21+I24</f>
         <v>2.0</v>
       </c>
-      <c r="J27" t="n" s="54">
+      <c r="J27" t="n" s="55">
         <f>J15+J18+J21+J24</f>
         <v>0.0</v>
       </c>
-      <c r="K27" t="n" s="54">
+      <c r="K27" t="n" s="55">
         <f>K15+K18+K21+K24</f>
-        <v>556.0</v>
-      </c>
-      <c r="L27" s="55" t="n">
+        <v>460.0</v>
+      </c>
+      <c r="L27" s="56" t="n">
         <f>L15+L18+L21+L24</f>
-        <v>11663.0</v>
-      </c>
-      <c r="M27" s="55" t="n">
+        <v>10027.0</v>
+      </c>
+      <c r="M27" s="56" t="n">
         <f>M15+M18+M21+M24</f>
-        <v>349.0</v>
-      </c>
-      <c r="N27" s="55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N27" s="56" t="n">
         <f>N15+N18+N21+N24</f>
         <v>0.0</v>
       </c>
-      <c r="O27" s="55" t="n">
+      <c r="O27" s="56" t="n">
         <f>O15+O18+O21+O24</f>
-        <v>220.0</v>
-      </c>
-      <c r="P27" s="55" t="n">
+        <v>540.0</v>
+      </c>
+      <c r="P27" s="56" t="n">
         <f>P15+P18+P21+P24</f>
         <v>0.0</v>
       </c>
-      <c r="Q27" s="55" t="n">
+      <c r="Q27" s="56" t="n">
         <f>Q15+Q18+Q21+Q24</f>
-        <v>3003.0</v>
-      </c>
-      <c r="R27" t="n" s="54">
+        <v>2507.0</v>
+      </c>
+      <c r="R27" t="n" s="55">
         <f>R15+R18+R21+R24</f>
         <v>0.0</v>
       </c>
-      <c r="S27" s="55" t="n">
+      <c r="S27" s="56" t="n">
         <f>S15+S18+S21+S24</f>
-        <v>754.0</v>
-      </c>
-      <c r="T27" s="55" t="n">
+        <v>574.0</v>
+      </c>
+      <c r="T27" s="56" t="n">
         <f>T15+T18+T21+T24</f>
         <v>0.0</v>
       </c>
-      <c r="U27" s="57"/>
+      <c r="U27" s="58"/>
     </row>
     <row r="28">
-      <c r="A28" s="49"/>
+      <c r="A28" s="50"/>
       <c r="E28" s="40" t="n">
         <f>E16+E19+E22+E25</f>
         <v>0.0</v>
@@ -2537,7 +2741,7 @@
       </c>
       <c r="L28" s="40" t="n">
         <f>L16+L19+L22+L25</f>
-        <v>0.0</v>
+        <v>1636.363525390625</v>
       </c>
       <c r="M28" s="40" t="n">
         <f>M16+M19+M22+M25</f>
@@ -2549,7 +2753,7 @@
       </c>
       <c r="O28" s="40" t="n">
         <f>O16+O19+O22+O25</f>
-        <v>12012.0</v>
+        <v>10027.0</v>
       </c>
       <c r="P28" s="40" t="n">
         <f>P16+P19+P22+P25</f>
@@ -2557,89 +2761,89 @@
       </c>
       <c r="Q28" s="40" t="n">
         <f>Q16+Q19+Q22+Q25</f>
-        <v>1167.0</v>
+        <v>1003.0</v>
       </c>
       <c r="R28" s="40" t="n">
         <f>R16+R19+R22+R25</f>
-        <v>7089.0</v>
+        <v>5943.0</v>
       </c>
       <c r="S28" s="40" t="n">
         <f>S16+S19+S22+S25</f>
-        <v>7089.0</v>
+        <v>5943.0</v>
       </c>
       <c r="T28" s="40" t="n">
         <f>T16+T19+T22+T25</f>
         <v>0.0</v>
       </c>
-      <c r="U28" s="51"/>
+      <c r="U28" s="52"/>
     </row>
     <row r="29">
-      <c r="A29" s="50"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="48" t="n">
+      <c r="A29" s="51"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="49" t="n">
         <f>D17+D20+D23+D26</f>
         <v>0.0</v>
       </c>
-      <c r="E29" s="48" t="n">
+      <c r="E29" s="49" t="n">
         <f>E17+E20+E23+E26</f>
         <v>0.0</v>
       </c>
-      <c r="F29" s="47" t="n">
+      <c r="F29" s="48" t="n">
         <f>F17+F20+F23+F26</f>
         <v>0.0</v>
       </c>
-      <c r="G29" s="47" t="n">
+      <c r="G29" s="48" t="n">
         <f>G17+G20+G23+G26</f>
-        <v>0.0</v>
-      </c>
-      <c r="H29" s="47" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H29" s="48" t="n">
         <f>H17+H20+H23+H26</f>
         <v>0.0</v>
       </c>
-      <c r="I29" s="47" t="n">
+      <c r="I29" s="48" t="n">
         <f>I17+I20+I23+I26</f>
         <v>0.0</v>
       </c>
-      <c r="J29" s="45"/>
-      <c r="K29" t="n" s="45">
+      <c r="J29" s="46"/>
+      <c r="K29" t="n" s="46">
         <f>K17+K20+K23+K26</f>
         <v>0.0</v>
       </c>
-      <c r="L29" t="n" s="45">
+      <c r="L29" t="n" s="46">
         <f>L17+L20+L23+L26</f>
         <v>0.0</v>
       </c>
-      <c r="M29" s="48" t="n">
+      <c r="M29" s="49" t="n">
         <f>N17+N20+N23+N26</f>
         <v>0.0</v>
       </c>
-      <c r="N29" s="45"/>
-      <c r="O29" t="n" s="45">
+      <c r="N29" s="46"/>
+      <c r="O29" t="n" s="46">
         <f>O17+O20+O23+O26</f>
         <v>0.0</v>
       </c>
-      <c r="P29" s="48" t="n">
+      <c r="P29" s="49" t="n">
         <f>P17+P20+P23+P26</f>
         <v>0.0</v>
       </c>
-      <c r="Q29" s="48" t="n">
+      <c r="Q29" s="49" t="n">
         <f>Q17+Q20+Q23+Q26</f>
-        <v>525.0</v>
-      </c>
-      <c r="R29" t="n" s="45">
+        <v>840.0</v>
+      </c>
+      <c r="R29" t="n" s="46">
         <f>R17+R20+R23+R26</f>
-        <v>0.0</v>
-      </c>
-      <c r="S29" s="48" t="n">
+        <v>5740.0</v>
+      </c>
+      <c r="S29" s="49" t="n">
         <f>S17+S20+S23+S26</f>
         <v>0.0</v>
       </c>
-      <c r="T29" s="48" t="n">
+      <c r="T29" s="49" t="n">
         <f>T17+T20+T23+T26</f>
-        <v>7089.0</v>
-      </c>
-      <c r="U29" s="52"/>
+        <v>5943.0</v>
+      </c>
+      <c r="U29" s="53"/>
     </row>
     <row r="30" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
@@ -2665,66 +2869,240 @@
       <c r="U30" s="39"/>
     </row>
     <row r="31">
-      <c r="A31" s="59" t="s">
+      <c r="A31" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="59" t="s">
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="J31" s="55"/>
+      <c r="K31" s="58"/>
+      <c r="M31" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="N31" s="55"/>
+      <c r="O31" s="55"/>
+      <c r="P31" s="58"/>
+      <c r="Q31" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="R31" s="55"/>
+      <c r="S31" s="58"/>
+      <c r="T31" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="U31" s="58"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="51"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="J32" s="46"/>
+      <c r="K32" s="53"/>
+      <c r="M32" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="N32" s="64"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="65"/>
+      <c r="Q32" s="51"/>
+      <c r="R32" s="46"/>
+      <c r="S32" s="53"/>
+      <c r="T32" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="U32" s="53"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="59" t="s">
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F33" s="64"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J33" s="64"/>
+      <c r="K33" s="65"/>
+      <c r="M33" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="N33" s="64"/>
+      <c r="O33" s="64"/>
+      <c r="P33" s="65"/>
+      <c r="Q33" s="63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R33" s="64"/>
+      <c r="S33" s="65"/>
+      <c r="T33" s="63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U33" s="65"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="J31" s="54"/>
-      <c r="K31" s="57"/>
-      <c r="M31" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="N31" s="54"/>
-      <c r="O31" s="54"/>
-      <c r="P31" s="57"/>
-      <c r="Q31" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="R31" s="54"/>
-      <c r="S31" s="57"/>
-      <c r="T31" s="59" t="s">
-        <v>90</v>
-      </c>
-      <c r="U31" s="57"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="50"/>
-      <c r="B32" s="45"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="61" t="s">
+      <c r="B34" s="64"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="68" t="n">
+        <v>10027.0</v>
+      </c>
+      <c r="F34" s="64"/>
+      <c r="G34" s="64"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="68" t="n">
+        <v>225.6075</v>
+      </c>
+      <c r="J34" s="64"/>
+      <c r="K34" s="65"/>
+      <c r="M34" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="N34" s="46"/>
+      <c r="O34" s="46"/>
+      <c r="P34" s="53"/>
+      <c r="Q34" s="63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R34" s="64"/>
+      <c r="S34" s="65"/>
+      <c r="T34" s="63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U34" s="65"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="J32" s="45"/>
-      <c r="K32" s="52"/>
-      <c r="M32" s="61" t="s">
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="68" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="68" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J35" s="64"/>
+      <c r="K35" s="65"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="N32" s="45"/>
-      <c r="O32" s="45"/>
-      <c r="P32" s="52"/>
-      <c r="Q32" s="50"/>
-      <c r="R32" s="45"/>
-      <c r="S32" s="52"/>
-      <c r="T32" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="U32" s="52"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="68" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="68" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J36" s="64"/>
+      <c r="K36" s="65"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" s="64"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="J38" s="64"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="M38" s="64"/>
+      <c r="N38" s="65"/>
+      <c r="O38" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="P38" s="64"/>
+      <c r="Q38" s="65"/>
+      <c r="R38" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="S38" s="64"/>
+      <c r="T38" s="65"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="B39" s="64"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="68" t="n">
+        <v>2507.0</v>
+      </c>
+      <c r="F39" s="64"/>
+      <c r="G39" s="64"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J39" s="64"/>
+      <c r="K39" s="65"/>
+      <c r="L39" s="68" t="n">
+        <v>574.0</v>
+      </c>
+      <c r="M39" s="64"/>
+      <c r="N39" s="65"/>
+      <c r="O39" s="63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P39" s="64"/>
+      <c r="Q39" s="65"/>
+      <c r="R39" s="63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S39" s="64"/>
+      <c r="T39" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="63">
@@ -2756,9 +3134,9 @@
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A35:D35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
     <mergeCell ref="E31:H31"/>
     <mergeCell ref="E33:H33"/>
     <mergeCell ref="E34:H34"/>

</xml_diff>

<commit_message>
scroll to top after recalcul/reset
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/downloads/Stat Salarii - Ingenio Software S.A. - Martie 2020.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/downloads/Stat Salarii - Ingenio Software S.A. - Martie 2020.xlsx
@@ -2509,7 +2509,7 @@
         <v>4958.0</v>
       </c>
       <c r="M24" s="56" t="n">
-        <v>0.0</v>
+        <v>349.0</v>
       </c>
       <c r="N24" s="56" t="n">
         <v>0.0</v>
@@ -2521,13 +2521,13 @@
         <v>0.0</v>
       </c>
       <c r="Q24" s="56" t="n">
-        <v>1240.0</v>
+        <v>1327.0</v>
       </c>
       <c r="R24" t="n" s="55">
         <v>0.0</v>
       </c>
       <c r="S24" s="56" t="n">
-        <v>322.0</v>
+        <v>348.0</v>
       </c>
       <c r="T24" s="56" t="n">
         <v>0.0</v>
@@ -2570,7 +2570,7 @@
         <v>0.0</v>
       </c>
       <c r="O25" s="40" t="n">
-        <v>4958.0</v>
+        <v>5307.0</v>
       </c>
       <c r="P25" s="40" t="n">
         <v>0.0</v>
@@ -2579,10 +2579,10 @@
         <v>496.0</v>
       </c>
       <c r="R25" s="40" t="n">
-        <v>2900.0</v>
+        <v>3136.0</v>
       </c>
       <c r="S25" t="n" s="40">
-        <v>2900.0</v>
+        <v>3136.0</v>
       </c>
       <c r="T25" s="40" t="n">
         <v>0.0</v>
@@ -2636,13 +2636,13 @@
         <v>0.0</v>
       </c>
       <c r="R26" t="n" s="46">
-        <v>3222.0</v>
+        <v>3484.0</v>
       </c>
       <c r="S26" t="n" s="46">
         <v>0.0</v>
       </c>
       <c r="T26" s="49" t="n">
-        <v>2900.0</v>
+        <v>3136.0</v>
       </c>
       <c r="U26" s="53"/>
     </row>
@@ -2681,7 +2681,7 @@
       </c>
       <c r="M27" s="56" t="n">
         <f>M15+M18+M21+M24</f>
-        <v>0.0</v>
+        <v>349.0</v>
       </c>
       <c r="N27" s="56" t="n">
         <f>N15+N18+N21+N24</f>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="Q27" s="56" t="n">
         <f>Q15+Q18+Q21+Q24</f>
-        <v>2507.0</v>
+        <v>2594.0</v>
       </c>
       <c r="R27" t="n" s="55">
         <f>R15+R18+R21+R24</f>
@@ -2705,7 +2705,7 @@
       </c>
       <c r="S27" s="56" t="n">
         <f>S15+S18+S21+S24</f>
-        <v>574.0</v>
+        <v>600.0</v>
       </c>
       <c r="T27" s="56" t="n">
         <f>T15+T18+T21+T24</f>
@@ -2753,7 +2753,7 @@
       </c>
       <c r="O28" s="40" t="n">
         <f>O16+O19+O22+O25</f>
-        <v>10027.0</v>
+        <v>10376.0</v>
       </c>
       <c r="P28" s="40" t="n">
         <f>P16+P19+P22+P25</f>
@@ -2765,11 +2765,11 @@
       </c>
       <c r="R28" s="40" t="n">
         <f>R16+R19+R22+R25</f>
-        <v>5943.0</v>
+        <v>6179.0</v>
       </c>
       <c r="S28" s="40" t="n">
         <f>S16+S19+S22+S25</f>
-        <v>5943.0</v>
+        <v>6179.0</v>
       </c>
       <c r="T28" s="40" t="n">
         <f>T16+T19+T22+T25</f>
@@ -2833,7 +2833,7 @@
       </c>
       <c r="R29" t="n" s="46">
         <f>R17+R20+R23+R26</f>
-        <v>5740.0</v>
+        <v>6002.0</v>
       </c>
       <c r="S29" s="49" t="n">
         <f>S17+S20+S23+S26</f>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="T29" s="49" t="n">
         <f>T17+T20+T23+T26</f>
-        <v>5943.0</v>
+        <v>6179.0</v>
       </c>
       <c r="U29" s="53"/>
     </row>
@@ -3078,7 +3078,7 @@
       <c r="C39" s="64"/>
       <c r="D39" s="65"/>
       <c r="E39" s="68" t="n">
-        <v>2507.0</v>
+        <v>2594.0</v>
       </c>
       <c r="F39" s="64"/>
       <c r="G39" s="64"/>
@@ -3089,7 +3089,7 @@
       <c r="J39" s="64"/>
       <c r="K39" s="65"/>
       <c r="L39" s="68" t="n">
-        <v>574.0</v>
+        <v>600.0</v>
       </c>
       <c r="M39" s="64"/>
       <c r="N39" s="65"/>

</xml_diff>